<commit_message>
Update Subscale - Bending and Barrowman Calcs.xlsx
</commit_message>
<xml_diff>
--- a/Subscale - Bending and Barrowman Calcs.xlsx
+++ b/Subscale - Bending and Barrowman Calcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kchee\OneDrive\Documents\Clubs and Fun\APRL Github\Vehicle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2350CEAA-0F5B-46A9-B30E-EC43F6781891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C41B536-C923-476D-91E9-FDA8DE59B9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{89B1A080-25E0-4FFB-AE02-629D748CE398}"/>
   </bookViews>
@@ -322,10 +322,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -4041,8 +4041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A825FAF-4742-4B1C-8FEE-CCCA86FED367}">
   <dimension ref="A1:AG85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AC46" sqref="AC46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4062,34 +4062,34 @@
       <c r="A1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="G1" s="6" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="O1" s="6" t="s">
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="O1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="S1" s="6" t="s">
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="S1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="X1" s="7" t="s">
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="X1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="Y1" s="7"/>
-      <c r="AB1" s="7" t="s">
+      <c r="Y1" s="6"/>
+      <c r="AB1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="AC1" s="7"/>
+      <c r="AC1" s="6"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
More updates to bending calcs
</commit_message>
<xml_diff>
--- a/Subscale - Bending and Barrowman Calcs.xlsx
+++ b/Subscale - Bending and Barrowman Calcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kchee\OneDrive\Documents\Clubs and Fun\APRL Github\Vehicle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51469378-A307-4E5C-B477-2D7FCEC71B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D960E851-CEF7-4E62-A5AF-9E842C5862DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{89B1A080-25E0-4FFB-AE02-629D748CE398}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="91">
   <si>
     <t>Calculation of Max Drag</t>
   </si>
@@ -231,13 +231,91 @@
   </si>
   <si>
     <t>You will also need to change the parts of the formula below the green cells that reference green cell values.</t>
+  </si>
+  <si>
+    <t>Compressive Stress Due to Drag (F_ca)</t>
+  </si>
+  <si>
+    <t>Outer Diameter</t>
+  </si>
+  <si>
+    <t>Inner Diameter</t>
+  </si>
+  <si>
+    <t>Ac</t>
+  </si>
+  <si>
+    <t>in^2</t>
+  </si>
+  <si>
+    <t>Section Modulus</t>
+  </si>
+  <si>
+    <t>Maximum Bending Stress</t>
+  </si>
+  <si>
+    <t>psi</t>
+  </si>
+  <si>
+    <t>D/t ratio</t>
+  </si>
+  <si>
+    <t>If D/t &gt; 70, use the graph below</t>
+  </si>
+  <si>
+    <t>L is the unsupported length of tube</t>
+  </si>
+  <si>
+    <t>Couplers can act as supports</t>
+  </si>
+  <si>
+    <t>For ultra-conservative, use entire length (not realistic)</t>
+  </si>
+  <si>
+    <t>Determining If Will Fail By Buckling</t>
+  </si>
+  <si>
+    <t>If below line, won't buckle</t>
+  </si>
+  <si>
+    <t>Max Combined Compressive Stress</t>
+  </si>
+  <si>
+    <t>Maximum Compressive Force</t>
+  </si>
+  <si>
+    <t>Figure from Richard Nakka Rocket Body Considerations</t>
+  </si>
+  <si>
+    <t>ONLY FOR ALUMINUM TUBES</t>
+  </si>
+  <si>
+    <t>Rocket Wet Mass (m)</t>
+  </si>
+  <si>
+    <t>Max Acceleration (a_max)</t>
+  </si>
+  <si>
+    <t>ft/s^2</t>
+  </si>
+  <si>
+    <t>Compressive  Stress Due to Mass Inertia</t>
+  </si>
+  <si>
+    <t>lbs</t>
+  </si>
+  <si>
+    <t>Safety Factor</t>
+  </si>
+  <si>
+    <t>Yield Stress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,8 +366,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,6 +384,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -311,11 +402,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -326,8 +418,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="40% - Accent5" xfId="2" builtinId="47"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3317,13 +3411,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>35</xdr:col>
+      <xdr:col>34</xdr:col>
       <xdr:colOff>21175</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>20106</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>49</xdr:col>
+      <xdr:col>48</xdr:col>
       <xdr:colOff>296333</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>105833</xdr:rowOff>
@@ -3353,13 +3447,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>35</xdr:col>
+      <xdr:col>34</xdr:col>
       <xdr:colOff>21167</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>49</xdr:col>
+      <xdr:col>48</xdr:col>
       <xdr:colOff>296333</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>22227</xdr:rowOff>
@@ -3391,13 +3485,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>35</xdr:col>
+      <xdr:col>34</xdr:col>
       <xdr:colOff>529168</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>63511</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>48</xdr:col>
+      <xdr:col>47</xdr:col>
       <xdr:colOff>74083</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>38129</xdr:rowOff>
@@ -3425,6 +3519,50 @@
         <a:xfrm>
           <a:off x="26670001" y="4254511"/>
           <a:ext cx="7524749" cy="546118"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>595312</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>66</xdr:col>
+      <xdr:colOff>414002</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>115326</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC1785E8-A7E7-9984-C2A0-3E799019A46B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38611968" y="1428750"/>
+          <a:ext cx="7105315" cy="4973076"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4039,10 +4177,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A825FAF-4742-4B1C-8FEE-CCCA86FED367}">
-  <dimension ref="A1:AG85"/>
+  <dimension ref="A1:BE85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AZ19" sqref="AZ19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4056,9 +4194,10 @@
     <col min="24" max="24" width="14.28515625" customWidth="1"/>
     <col min="27" max="27" width="12.42578125" customWidth="1"/>
     <col min="28" max="28" width="14.42578125" customWidth="1"/>
+    <col min="52" max="52" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -4090,8 +4229,14 @@
         <v>54</v>
       </c>
       <c r="AC1" s="6"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AZ1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="BD1" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
@@ -4121,8 +4266,24 @@
       </c>
       <c r="X2" s="4"/>
       <c r="AB2" s="4"/>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AZ2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BA2">
+        <v>3.12</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>13</v>
+      </c>
+      <c r="BD2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="BE2">
+        <f>BA2/((BA2-BA3)/2)</f>
+        <v>51.999999999999957</v>
+      </c>
+    </row>
+    <row r="3" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -4175,8 +4336,20 @@
       <c r="AC3" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AZ3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BA3">
+        <v>3</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>13</v>
+      </c>
+      <c r="BD3" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>34</v>
       </c>
@@ -4234,8 +4407,22 @@
         <f>$H$25*AB4-(0.5*$T$9*(AB4*AB4))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AZ4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="BA4">
+        <f>(PI()/4)*(BA2^2-BA3^2)</f>
+        <v>0.57679641119908664</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>69</v>
+      </c>
+      <c r="BD4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="BE4" s="3"/>
+    </row>
+    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>31</v>
       </c>
@@ -4298,8 +4485,22 @@
         <f>$H$25*AB5-(0.5*$T$9*(AB5*AB5))</f>
         <v>21.205717540720702</v>
       </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AZ5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="BA5">
+        <f>D7/BA4</f>
+        <v>27.129574267700015</v>
+      </c>
+      <c r="BB5" t="s">
+        <v>72</v>
+      </c>
+      <c r="BD5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="BE5" s="3"/>
+    </row>
+    <row r="6" spans="1:57" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
@@ -4338,8 +4539,12 @@
         <f t="shared" ref="AC6:AC44" si="5">$H$25*AB6-(0.5*$T$9*(AB6*AB6))</f>
         <v>41.769796457491324</v>
       </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="BD6" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="BE6" s="3"/>
+    </row>
+    <row r="7" spans="1:57" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
@@ -4389,8 +4594,19 @@
         <f t="shared" si="5"/>
         <v>61.692236750311878</v>
       </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AZ7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="BA7">
+        <f>(PI()/(32*BA2)*(BA2^4-BA3^4))</f>
+        <v>0.43293007555962221</v>
+      </c>
+      <c r="BD7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="BE7" s="3"/>
+    </row>
+    <row r="8" spans="1:57" x14ac:dyDescent="0.25">
       <c r="G8" s="1" t="s">
         <v>30</v>
       </c>
@@ -4440,8 +4656,18 @@
         <f t="shared" si="5"/>
         <v>80.973038419182359</v>
       </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AZ8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA8">
+        <f>MAX(AC4:AC85)/BA7</f>
+        <v>833.9340432327881</v>
+      </c>
+      <c r="BB8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:57" x14ac:dyDescent="0.25">
       <c r="G9" s="1" t="s">
         <v>31</v>
       </c>
@@ -4496,7 +4722,7 @@
         <v>99.612201464102768</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:57" x14ac:dyDescent="0.25">
       <c r="G10" s="1" t="s">
         <v>16</v>
       </c>
@@ -4530,8 +4756,17 @@
         <f t="shared" si="5"/>
         <v>117.60972588507309</v>
       </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AZ10" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BA10">
+        <v>601</v>
+      </c>
+      <c r="BB10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:57" x14ac:dyDescent="0.25">
       <c r="G11" s="1" t="s">
         <v>17</v>
       </c>
@@ -4575,8 +4810,17 @@
         <f t="shared" si="5"/>
         <v>134.96561168209337</v>
       </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AZ11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BA11">
+        <v>18.1875</v>
+      </c>
+      <c r="BB11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:57" x14ac:dyDescent="0.25">
       <c r="G12" s="1" t="s">
         <v>18</v>
       </c>
@@ -4610,8 +4854,18 @@
         <f t="shared" si="5"/>
         <v>151.67985885516353</v>
       </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AZ12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BA12">
+        <f>(BA11*32.2*(1+(BA10/32/2))/BA4)</f>
+        <v>10549.891660711388</v>
+      </c>
+      <c r="BB12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:57" x14ac:dyDescent="0.25">
       <c r="G13" s="1" t="s">
         <v>19</v>
       </c>
@@ -4646,7 +4900,7 @@
         <v>167.75246740428364</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:57" x14ac:dyDescent="0.25">
       <c r="G14" s="1" t="s">
         <v>20</v>
       </c>
@@ -4680,8 +4934,18 @@
         <f t="shared" si="5"/>
         <v>183.18343732945368</v>
       </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AZ14" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="BA14" s="8">
+        <f>BA5+BA8+BA12</f>
+        <v>11410.955278211875</v>
+      </c>
+      <c r="BB14" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:57" x14ac:dyDescent="0.25">
       <c r="G15" s="2" t="s">
         <v>21</v>
       </c>
@@ -4717,7 +4981,7 @@
         <v>197.97276863067361</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:57" x14ac:dyDescent="0.25">
       <c r="G16" s="2" t="s">
         <v>22</v>
       </c>
@@ -4752,8 +5016,17 @@
         <f t="shared" si="5"/>
         <v>212.12046130794351</v>
       </c>
-    </row>
-    <row r="17" spans="7:29" x14ac:dyDescent="0.25">
+      <c r="AZ16" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BA16">
+        <v>35000</v>
+      </c>
+      <c r="BB16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="7:53" x14ac:dyDescent="0.25">
       <c r="G17" s="2" t="s">
         <v>36</v>
       </c>
@@ -4788,8 +5061,15 @@
         <f t="shared" si="5"/>
         <v>225.62651536126333</v>
       </c>
-    </row>
-    <row r="18" spans="7:29" x14ac:dyDescent="0.25">
+      <c r="AZ17" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="BA17" s="8">
+        <f>BA16/BA14</f>
+        <v>3.0672278653855689</v>
+      </c>
+    </row>
+    <row r="18" spans="7:53" x14ac:dyDescent="0.25">
       <c r="W18">
         <f t="shared" si="0"/>
         <v>21.5</v>
@@ -4815,7 +5095,7 @@
         <v>238.49093079063309</v>
       </c>
     </row>
-    <row r="19" spans="7:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:53" x14ac:dyDescent="0.25">
       <c r="G19" s="2" t="s">
         <v>25</v>
       </c>
@@ -4851,7 +5131,7 @@
         <v>250.7137075960527</v>
       </c>
     </row>
-    <row r="20" spans="7:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="7:53" x14ac:dyDescent="0.25">
       <c r="W20">
         <f t="shared" si="0"/>
         <v>23.5</v>
@@ -4877,7 +5157,7 @@
         <v>262.29484577752231</v>
       </c>
     </row>
-    <row r="21" spans="7:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="7:53" x14ac:dyDescent="0.25">
       <c r="W21">
         <f t="shared" si="0"/>
         <v>24.5</v>
@@ -4903,7 +5183,7 @@
         <v>273.23434533504184</v>
       </c>
     </row>
-    <row r="22" spans="7:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="7:53" x14ac:dyDescent="0.25">
       <c r="G22" t="s">
         <v>26</v>
       </c>
@@ -4932,7 +5212,7 @@
         <v>283.53220626861128</v>
       </c>
     </row>
-    <row r="23" spans="7:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="7:53" x14ac:dyDescent="0.25">
       <c r="G23" t="s">
         <v>43</v>
       </c>
@@ -4964,7 +5244,7 @@
         <v>293.18842857823063</v>
       </c>
     </row>
-    <row r="24" spans="7:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="7:53" x14ac:dyDescent="0.25">
       <c r="G24" s="1" t="s">
         <v>36</v>
       </c>
@@ -4999,7 +5279,7 @@
         <v>302.20301226389995</v>
       </c>
     </row>
-    <row r="25" spans="7:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="7:53" x14ac:dyDescent="0.25">
       <c r="G25" s="2" t="s">
         <v>44</v>
       </c>
@@ -5035,7 +5315,7 @@
         <v>310.57595732561913</v>
       </c>
     </row>
-    <row r="26" spans="7:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="7:53" x14ac:dyDescent="0.25">
       <c r="W26">
         <f t="shared" si="0"/>
         <v>29.5</v>
@@ -5061,7 +5341,7 @@
         <v>318.30726376338828</v>
       </c>
     </row>
-    <row r="27" spans="7:29" x14ac:dyDescent="0.25">
+    <row r="27" spans="7:53" x14ac:dyDescent="0.25">
       <c r="W27">
         <f t="shared" si="0"/>
         <v>30.5</v>
@@ -5087,7 +5367,7 @@
         <v>325.3969315772074</v>
       </c>
     </row>
-    <row r="28" spans="7:29" x14ac:dyDescent="0.25">
+    <row r="28" spans="7:53" x14ac:dyDescent="0.25">
       <c r="W28">
         <f t="shared" si="0"/>
         <v>31.5</v>
@@ -5113,7 +5393,7 @@
         <v>331.84496076707632</v>
       </c>
     </row>
-    <row r="29" spans="7:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="7:53" x14ac:dyDescent="0.25">
       <c r="W29">
         <f t="shared" si="0"/>
         <v>32.5</v>
@@ -5139,7 +5419,7 @@
         <v>337.65135133299532</v>
       </c>
     </row>
-    <row r="30" spans="7:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="7:53" x14ac:dyDescent="0.25">
       <c r="W30">
         <f t="shared" si="0"/>
         <v>33.5</v>
@@ -5165,7 +5445,7 @@
         <v>342.81610327496412</v>
       </c>
     </row>
-    <row r="31" spans="7:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="7:53" x14ac:dyDescent="0.25">
       <c r="W31">
         <f t="shared" si="0"/>
         <v>34.5</v>
@@ -5191,7 +5471,7 @@
         <v>347.33921659298284</v>
       </c>
     </row>
-    <row r="32" spans="7:29" x14ac:dyDescent="0.25">
+    <row r="32" spans="7:53" x14ac:dyDescent="0.25">
       <c r="W32">
         <f t="shared" si="0"/>
         <v>35.5</v>
@@ -5217,7 +5497,7 @@
         <v>351.22069128705164</v>
       </c>
     </row>
-    <row r="33" spans="23:33" x14ac:dyDescent="0.25">
+    <row r="33" spans="23:56" x14ac:dyDescent="0.25">
       <c r="W33">
         <f t="shared" si="0"/>
         <v>36.5</v>
@@ -5243,7 +5523,7 @@
         <v>354.46052735717018</v>
       </c>
     </row>
-    <row r="34" spans="23:33" x14ac:dyDescent="0.25">
+    <row r="34" spans="23:56" x14ac:dyDescent="0.25">
       <c r="W34">
         <f t="shared" si="0"/>
         <v>37.5</v>
@@ -5269,7 +5549,7 @@
         <v>357.05872480333869</v>
       </c>
     </row>
-    <row r="35" spans="23:33" x14ac:dyDescent="0.25">
+    <row r="35" spans="23:56" x14ac:dyDescent="0.25">
       <c r="W35">
         <f t="shared" si="0"/>
         <v>38.5</v>
@@ -5294,8 +5574,11 @@
         <f t="shared" si="5"/>
         <v>359.01528362555729</v>
       </c>
-    </row>
-    <row r="36" spans="23:33" x14ac:dyDescent="0.25">
+      <c r="BD35" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="23:56" x14ac:dyDescent="0.25">
       <c r="W36">
         <f t="shared" si="0"/>
         <v>39.5</v>
@@ -5320,8 +5603,11 @@
         <f t="shared" si="5"/>
         <v>360.33020382382563</v>
       </c>
-    </row>
-    <row r="37" spans="23:33" x14ac:dyDescent="0.25">
+      <c r="BD36" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="23:56" x14ac:dyDescent="0.25">
       <c r="W37">
         <f t="shared" si="0"/>
         <v>40.5</v>
@@ -5347,7 +5633,7 @@
         <v>361.00348539814394</v>
       </c>
     </row>
-    <row r="38" spans="23:33" x14ac:dyDescent="0.25">
+    <row r="38" spans="23:56" x14ac:dyDescent="0.25">
       <c r="W38">
         <f t="shared" si="0"/>
         <v>41.5</v>
@@ -5373,7 +5659,7 @@
         <v>361.03512834851222</v>
       </c>
     </row>
-    <row r="39" spans="23:33" x14ac:dyDescent="0.25">
+    <row r="39" spans="23:56" x14ac:dyDescent="0.25">
       <c r="W39">
         <f t="shared" si="0"/>
         <v>42.5</v>
@@ -5399,7 +5685,7 @@
         <v>360.42513267493035</v>
       </c>
     </row>
-    <row r="40" spans="23:33" x14ac:dyDescent="0.25">
+    <row r="40" spans="23:56" x14ac:dyDescent="0.25">
       <c r="W40">
         <f t="shared" si="0"/>
         <v>43.5</v>
@@ -5425,7 +5711,7 @@
         <v>359.17349837739846</v>
       </c>
     </row>
-    <row r="41" spans="23:33" x14ac:dyDescent="0.25">
+    <row r="41" spans="23:56" x14ac:dyDescent="0.25">
       <c r="W41">
         <f t="shared" si="0"/>
         <v>44.5</v>
@@ -5451,7 +5737,7 @@
         <v>357.28022545591654</v>
       </c>
     </row>
-    <row r="42" spans="23:33" x14ac:dyDescent="0.25">
+    <row r="42" spans="23:56" x14ac:dyDescent="0.25">
       <c r="W42">
         <f t="shared" si="0"/>
         <v>45.5</v>
@@ -5477,7 +5763,7 @@
         <v>354.74531391048447</v>
       </c>
     </row>
-    <row r="43" spans="23:33" x14ac:dyDescent="0.25">
+    <row r="43" spans="23:56" x14ac:dyDescent="0.25">
       <c r="W43">
         <f t="shared" si="0"/>
         <v>46.5</v>
@@ -5503,7 +5789,7 @@
         <v>351.56876374110232</v>
       </c>
     </row>
-    <row r="44" spans="23:33" x14ac:dyDescent="0.25">
+    <row r="44" spans="23:56" x14ac:dyDescent="0.25">
       <c r="W44">
         <f t="shared" si="0"/>
         <v>46.978000000000002</v>
@@ -5534,7 +5820,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="23:33" x14ac:dyDescent="0.25">
+    <row r="45" spans="23:56" x14ac:dyDescent="0.25">
       <c r="W45">
         <f t="shared" si="0"/>
         <v>47.5</v>
@@ -5566,7 +5852,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="23:33" x14ac:dyDescent="0.25">
+    <row r="46" spans="23:56" x14ac:dyDescent="0.25">
       <c r="W46">
         <f t="shared" si="0"/>
         <v>48.5</v>
@@ -5592,7 +5878,7 @@
         <v>343.74666080100354</v>
       </c>
     </row>
-    <row r="47" spans="23:33" x14ac:dyDescent="0.25">
+    <row r="47" spans="23:56" x14ac:dyDescent="0.25">
       <c r="W47">
         <f t="shared" si="0"/>
         <v>49.5</v>
@@ -5618,7 +5904,7 @@
         <v>339.44110496936736</v>
       </c>
     </row>
-    <row r="48" spans="23:33" x14ac:dyDescent="0.25">
+    <row r="48" spans="23:56" x14ac:dyDescent="0.25">
       <c r="W48">
         <f t="shared" si="0"/>
         <v>50.5</v>

</xml_diff>